<commit_message>
Start case series data extraction
</commit_message>
<xml_diff>
--- a/input/raw_data/data_extraction/case_report_data_extraction_end.xlsx
+++ b/input/raw_data/data_extraction/case_report_data_extraction_end.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Library/Mobile Documents/com~apple~CloudDocs/Dev/data/msc/dissertation/iifo_data/lit_search_4/input/raw_data/data_extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/data_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5C511B-21E6-AF49-9AFE-81ED68AB8641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{223AB0F5-CC98-3A4D-88E5-62BC8261968D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20540" yWindow="880" windowWidth="20580" windowHeight="12220" xr2:uid="{75954437-E4AF-7C43-AD2A-639C66837574}"/>
+    <workbookView xWindow="19520" yWindow="880" windowWidth="20580" windowHeight="12220" xr2:uid="{75954437-E4AF-7C43-AD2A-639C66837574}"/>
   </bookViews>
   <sheets>
     <sheet name="case_report_data_extraction" sheetId="1" r:id="rId1"/>
@@ -2174,8 +2174,8 @@
   <dimension ref="A1:AH110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z110" sqref="Z110"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>